<commit_message>
Aptitude project with Bootstrap
</commit_message>
<xml_diff>
--- a/public/Student.xlsx
+++ b/public/Student.xlsx
@@ -97,14 +97,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="36.08988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.58988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="20.68988764044944"/>
   </cols>
   <sheetData>
@@ -128,51 +128,34 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Who invented Ruby </t>
+          <t>What is the acronym of PHP</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Yukihiro Matsumoto</t>
+          <t>Hypertext Preprocessor</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Yukihiro Matsumoto</t>
+          <t>Preprocessor Hypertext Page</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>How do you write to STDOUT in Ruby?</t>
+          <t>Which is the current stable version of php</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>puts</t>
+          <t>Php-5.5.9</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>puts</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>Who invented Rails</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>David Heinemeier Hansson</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>David Heinemeier Hansson</t>
+          <t>Php-5.4.5</t>
         </is>
       </c>
     </row>

</xml_diff>